<commit_message>
Add help feature with modal for test case details - Add question mark button next to each test case - Implement modal window to display Steps and Expected Output - Change Actions column header to Details - Update backend to read steps and Expected Output columns from Excel - Improve UI/UX with clean modal design and proper formatting
</commit_message>
<xml_diff>
--- a/backend/data/test_cases.xlsx
+++ b/backend/data/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhilreddy/Desktop/test-management-system/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38722D5B-3F9B-D440-B15D-3EAC4F98AA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2FA812-20A5-A448-B51C-F700E3BCA9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="16260" xr2:uid="{2CCD88E7-89DF-7944-A495-39644DA0F665}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="90">
   <si>
     <t>Test Case</t>
   </si>
@@ -272,13 +272,46 @@
   </si>
   <si>
     <t>Phase 2</t>
+  </si>
+  <si>
+    <t>XIB</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>TEST - 101</t>
+  </si>
+  <si>
+    <t>Hardening</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>vhierfhewusnjiuefbarbcj. H uauhiufheriua</t>
+  </si>
+  <si>
+    <t>reyghvbierbverui</t>
+  </si>
+  <si>
+    <t>tgiuryebflve</t>
+  </si>
+  <si>
+    <t>etbrgvewfvrve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -295,6 +328,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -320,9 +360,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84547CFC-C1BD-454E-BE95-B41DF2AC9D8C}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,9 +690,11 @@
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -666,8 +710,14 @@
       <c r="E1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -683,8 +733,14 @@
       <c r="E2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -700,8 +756,14 @@
       <c r="E3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -717,8 +779,14 @@
       <c r="E4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -734,8 +802,14 @@
       <c r="E5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -751,8 +825,14 @@
       <c r="E6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -768,8 +848,14 @@
       <c r="E7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -785,8 +871,14 @@
       <c r="E8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -802,8 +894,14 @@
       <c r="E9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -819,8 +917,14 @@
       <c r="E10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -831,13 +935,19 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -848,13 +958,19 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -865,13 +981,19 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -882,13 +1004,19 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -904,8 +1032,14 @@
       <c r="E15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -921,8 +1055,14 @@
       <c r="E16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -938,8 +1078,14 @@
       <c r="E17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -955,8 +1101,14 @@
       <c r="E18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -972,8 +1124,14 @@
       <c r="E19" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -989,8 +1147,14 @@
       <c r="E20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1006,8 +1170,14 @@
       <c r="E21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1023,8 +1193,14 @@
       <c r="E22" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1040,8 +1216,14 @@
       <c r="E23" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1057,8 +1239,14 @@
       <c r="E24" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1074,8 +1262,14 @@
       <c r="E25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1086,13 +1280,19 @@
         <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1103,13 +1303,19 @@
         <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1120,13 +1326,19 @@
         <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1137,13 +1349,19 @@
         <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1159,8 +1377,14 @@
       <c r="E30" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1176,8 +1400,14 @@
       <c r="E31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1193,8 +1423,14 @@
       <c r="E32" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1210,8 +1446,14 @@
       <c r="E33" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1227,8 +1469,14 @@
       <c r="E34" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1244,8 +1492,14 @@
       <c r="E35" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1261,8 +1515,14 @@
       <c r="E36" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1278,8 +1538,14 @@
       <c r="E37" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1295,8 +1561,14 @@
       <c r="E38" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1307,13 +1579,19 @@
         <v>32</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E39" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1324,13 +1602,19 @@
         <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E40" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1341,13 +1625,19 @@
         <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E41" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1358,13 +1648,19 @@
         <v>31</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E42" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1380,8 +1676,14 @@
       <c r="E43" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1397,8 +1699,14 @@
       <c r="E44" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1414,8 +1722,14 @@
       <c r="E45" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1431,8 +1745,14 @@
       <c r="E46" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1448,8 +1768,14 @@
       <c r="E47" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1465,8 +1791,14 @@
       <c r="E48" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1482,8 +1814,14 @@
       <c r="E49" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1499,8 +1837,14 @@
       <c r="E50" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1516,8 +1860,14 @@
       <c r="E51" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -1528,13 +1878,19 @@
         <v>32</v>
       </c>
       <c r="D52" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E52" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -1545,13 +1901,19 @@
         <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E53" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -1562,13 +1924,19 @@
         <v>34</v>
       </c>
       <c r="D54" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E54" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -1579,11 +1947,516 @@
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E55" t="s">
         <v>75</v>
       </c>
+      <c r="F55" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" t="s">
+        <v>75</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+    </row>
+    <row r="88" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+    </row>
+    <row r="89" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+    </row>
+    <row r="90" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+    </row>
+    <row r="96" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+    </row>
+    <row r="97" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+    </row>
+    <row r="98" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+    </row>
+    <row r="99" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+    </row>
+    <row r="100" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+    </row>
+    <row r="101" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+    </row>
+    <row r="103" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+    </row>
+    <row r="104" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+    </row>
+    <row r="105" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+    </row>
+    <row r="106" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+    </row>
+    <row r="107" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+    </row>
+    <row r="108" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+    </row>
+    <row r="109" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+    </row>
+    <row r="110" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+    </row>
+    <row r="111" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+    </row>
+    <row r="112" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+    </row>
+    <row r="113" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+    </row>
+    <row r="114" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+    </row>
+    <row r="115" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+    </row>
+    <row r="116" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+    </row>
+    <row r="117" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+    </row>
+    <row r="118" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+    </row>
+    <row r="119" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+    </row>
+    <row r="120" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+    </row>
+    <row r="121" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+    </row>
+    <row r="122" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+    </row>
+    <row r="123" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+    </row>
+    <row r="124" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+    </row>
+    <row r="125" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+    </row>
+    <row r="126" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+    </row>
+    <row r="127" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+    </row>
+    <row r="128" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+    </row>
+    <row r="129" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+    </row>
+    <row r="131" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+    </row>
+    <row r="132" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+    </row>
+    <row r="133" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+    </row>
+    <row r="134" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+    </row>
+    <row r="135" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+    </row>
+    <row r="136" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+    </row>
+    <row r="137" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+    </row>
+    <row r="138" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+    </row>
+    <row r="139" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+    </row>
+    <row r="140" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+    </row>
+    <row r="141" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+    </row>
+    <row r="142" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+    </row>
+    <row r="143" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+    </row>
+    <row r="144" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+    </row>
+    <row r="145" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+    </row>
+    <row r="146" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+    </row>
+    <row r="147" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+    </row>
+    <row r="148" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+    </row>
+    <row r="149" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+    </row>
+    <row r="150" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+    </row>
+    <row r="151" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+    </row>
+    <row r="152" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+    </row>
+    <row r="153" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F153" s="2"/>
+      <c r="G153" s="2"/>
+    </row>
+    <row r="154" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+    </row>
+    <row r="155" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+    </row>
+    <row r="156" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+    </row>
+    <row r="157" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+    </row>
+    <row r="158" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+    </row>
+    <row r="159" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F159" s="2"/>
+      <c r="G159" s="2"/>
+    </row>
+    <row r="160" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+    </row>
+    <row r="161" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+    </row>
+    <row r="162" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F162" s="2"/>
+      <c r="G162" s="2"/>
+    </row>
+    <row r="163" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F163" s="2"/>
+      <c r="G163" s="2"/>
+    </row>
+    <row r="164" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F164" s="2"/>
+      <c r="G164" s="2"/>
+    </row>
+    <row r="165" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+    </row>
+    <row r="166" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+    </row>
+    <row r="167" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F167" s="2"/>
+      <c r="G167" s="2"/>
+    </row>
+    <row r="168" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F168" s="2"/>
+      <c r="G168" s="2"/>
+    </row>
+    <row r="169" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F169" s="2"/>
+      <c r="G169" s="2"/>
+    </row>
+    <row r="170" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F170" s="2"/>
+      <c r="G170" s="2"/>
+    </row>
+    <row r="171" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F171" s="2"/>
+      <c r="G171" s="2"/>
+    </row>
+    <row r="172" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F172" s="2"/>
+      <c r="G172" s="2"/>
+    </row>
+    <row r="173" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F173" s="2"/>
+      <c r="G173" s="2"/>
+    </row>
+    <row r="174" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F174" s="2"/>
+      <c r="G174" s="2"/>
+    </row>
+    <row r="175" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F175" s="2"/>
+      <c r="G175" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Fix steps column name to match Excel file - Update backend to read 'Steps' column (capital S) instead of 'steps' - Fix column name consistency between Excel file and backend code - Enable help modal to display both Steps and Expected Output data
</commit_message>
<xml_diff>
--- a/backend/data/test_cases.xlsx
+++ b/backend/data/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhilreddy/Desktop/test-management-system/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2FA812-20A5-A448-B51C-F700E3BCA9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875CC54B-0A83-5148-BF21-0A3F2D59D638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="16260" xr2:uid="{2CCD88E7-89DF-7944-A495-39644DA0F665}"/>
   </bookViews>
@@ -364,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,7 +682,7 @@
   <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G56"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>